<commit_message>
update for the blank test data
</commit_message>
<xml_diff>
--- a/test/_qaf-bdd-syntax/testdata/testdata.xlsx
+++ b/test/_qaf-bdd-syntax/testdata/testdata.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="15660" tabRatio="664" firstSheet="1" activeTab="8"/>
+    <workbookView windowHeight="15620" tabRatio="664" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="FirstSheet" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="84">
   <si>
     <t>Id</t>
   </si>
@@ -2708,7 +2708,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17.6" outlineLevelRow="3" outlineLevelCol="2"/>
@@ -2746,10 +2746,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>83</v>
-      </c>
+    <row r="4" spans="2:3">
       <c r="B4" s="1">
         <v>4</v>
       </c>

</xml_diff>